<commit_message>
Added e-mail address to excel file
</commit_message>
<xml_diff>
--- a/template_examples/rna_expression.xlsx
+++ b/template_examples/rna_expression.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="27220" windowHeight="11780"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="29160" windowHeight="15920"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0">
+    <comment ref="B10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>User's preferred email address.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0">
+    <comment ref="C13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -162,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0">
+    <comment ref="D13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -175,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0">
+    <comment ref="E13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -188,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0">
+    <comment ref="F13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -201,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0">
+    <comment ref="G13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -214,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H12" authorId="0">
+    <comment ref="H13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -227,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0">
+    <comment ref="I13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -240,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J12" authorId="0">
+    <comment ref="J13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -253,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K12" authorId="0">
+    <comment ref="K13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -266,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L12" authorId="0">
+    <comment ref="L13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -279,7 +292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M12" authorId="0">
+    <comment ref="M13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -292,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N12" authorId="0">
+    <comment ref="N13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -310,7 +323,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="43">
   <si>
     <t>#t</t>
   </si>
@@ -345,6 +358,9 @@
     <t>LEAD ORGANIZATION STUDY ID</t>
   </si>
   <si>
+    <t>EMAIL ADDRESS</t>
+  </si>
+  <si>
     <t>Samples</t>
   </si>
   <si>
@@ -411,22 +427,25 @@
     <t>Single</t>
   </si>
   <si>
-    <t>Study 2</t>
-  </si>
-  <si>
-    <t>Patient A</t>
-  </si>
-  <si>
-    <t>Aliquot B</t>
+    <t>another study</t>
+  </si>
+  <si>
+    <t>mducar@partners.org</t>
+  </si>
+  <si>
+    <t>Patient 2</t>
+  </si>
+  <si>
+    <t>aliquot 1</t>
   </si>
   <si>
     <t>Tumor</t>
   </si>
   <si>
-    <t>Lot 1</t>
-  </si>
-  <si>
-    <t>Lot Z</t>
+    <t>lot 987</t>
+  </si>
+  <si>
+    <t>lot 543</t>
   </si>
   <si>
     <t>gs://path/to/fwd.fastq</t>
@@ -439,7 +458,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,6 +479,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -523,10 +550,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -537,9 +565,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -839,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N212"/>
+  <dimension ref="A1:N213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -879,7 +911,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -901,7 +933,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -923,7 +955,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -945,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -967,7 +999,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -989,7 +1021,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1033,7 +1065,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1047,1107 +1079,1129 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="4">
-        <v>43590</v>
-      </c>
-      <c r="H13" s="4">
-        <v>43588</v>
-      </c>
-      <c r="I13">
-        <v>225</v>
-      </c>
-      <c r="J13">
-        <v>885</v>
-      </c>
-      <c r="K13">
-        <v>100</v>
-      </c>
-      <c r="L13" t="s">
-        <v>39</v>
-      </c>
-      <c r="N13" t="s">
-        <v>40</v>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="5">
+        <v>43588</v>
+      </c>
+      <c r="H14" s="5">
+        <v>43586</v>
+      </c>
+      <c r="I14">
+        <v>100</v>
+      </c>
+      <c r="J14">
+        <v>650</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="L14" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:N1"/>
-    <mergeCell ref="B11:N11"/>
+    <mergeCell ref="B12:N12"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
@@ -2165,17 +2219,20 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
       <formula1>"Paired,Single"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:D212">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D213">
       <formula1>"Tumor,Normal,Metastasis"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G13:G212">
-      <formula1>AND(ISNUMBER(G13:G212),LEFT(CELL("format",G13:G212),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G14:G213">
+      <formula1>AND(ISNUMBER(G14:G213),LEFT(CELL("format",G14:G213),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="H13:H212">
-      <formula1>AND(ISNUMBER(H13:H212),LEFT(CELL("format",H13:H212),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="H14:H213">
+      <formula1>AND(ISNUMBER(H14:H213),LEFT(CELL("format",H14:H213),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added e-mail address to excel file (#41)
</commit_message>
<xml_diff>
--- a/template_examples/rna_expression.xlsx
+++ b/template_examples/rna_expression.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="27220" windowHeight="11780"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="29160" windowHeight="15920"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0">
+    <comment ref="B10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>User's preferred email address.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0">
+    <comment ref="C13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -162,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0">
+    <comment ref="D13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -175,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0">
+    <comment ref="E13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -188,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0">
+    <comment ref="F13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -201,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0">
+    <comment ref="G13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -214,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H12" authorId="0">
+    <comment ref="H13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -227,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0">
+    <comment ref="I13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -240,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J12" authorId="0">
+    <comment ref="J13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -253,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K12" authorId="0">
+    <comment ref="K13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -266,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L12" authorId="0">
+    <comment ref="L13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -279,7 +292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M12" authorId="0">
+    <comment ref="M13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -292,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N12" authorId="0">
+    <comment ref="N13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -310,7 +323,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="43">
   <si>
     <t>#t</t>
   </si>
@@ -345,6 +358,9 @@
     <t>LEAD ORGANIZATION STUDY ID</t>
   </si>
   <si>
+    <t>EMAIL ADDRESS</t>
+  </si>
+  <si>
     <t>Samples</t>
   </si>
   <si>
@@ -411,22 +427,25 @@
     <t>Single</t>
   </si>
   <si>
-    <t>Study 2</t>
-  </si>
-  <si>
-    <t>Patient A</t>
-  </si>
-  <si>
-    <t>Aliquot B</t>
+    <t>another study</t>
+  </si>
+  <si>
+    <t>mducar@partners.org</t>
+  </si>
+  <si>
+    <t>Patient 2</t>
+  </si>
+  <si>
+    <t>aliquot 1</t>
   </si>
   <si>
     <t>Tumor</t>
   </si>
   <si>
-    <t>Lot 1</t>
-  </si>
-  <si>
-    <t>Lot Z</t>
+    <t>lot 987</t>
+  </si>
+  <si>
+    <t>lot 543</t>
   </si>
   <si>
     <t>gs://path/to/fwd.fastq</t>
@@ -439,7 +458,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,6 +479,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -523,10 +550,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -537,9 +565,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -839,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N212"/>
+  <dimension ref="A1:N213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -879,7 +911,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -901,7 +933,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -923,7 +955,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -945,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -967,7 +999,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -989,7 +1021,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1033,7 +1065,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1047,1107 +1079,1129 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="4">
-        <v>43590</v>
-      </c>
-      <c r="H13" s="4">
-        <v>43588</v>
-      </c>
-      <c r="I13">
-        <v>225</v>
-      </c>
-      <c r="J13">
-        <v>885</v>
-      </c>
-      <c r="K13">
-        <v>100</v>
-      </c>
-      <c r="L13" t="s">
-        <v>39</v>
-      </c>
-      <c r="N13" t="s">
-        <v>40</v>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="5">
+        <v>43588</v>
+      </c>
+      <c r="H14" s="5">
+        <v>43586</v>
+      </c>
+      <c r="I14">
+        <v>100</v>
+      </c>
+      <c r="J14">
+        <v>650</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="L14" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:N1"/>
-    <mergeCell ref="B11:N11"/>
+    <mergeCell ref="B12:N12"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
@@ -2165,17 +2219,20 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
       <formula1>"Paired,Single"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:D212">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D213">
       <formula1>"Tumor,Normal,Metastasis"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G13:G212">
-      <formula1>AND(ISNUMBER(G13:G212),LEFT(CELL("format",G13:G212),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="G14:G213">
+      <formula1>AND(ISNUMBER(G14:G213),LEFT(CELL("format",G14:G213),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="H13:H212">
-      <formula1>AND(ISNUMBER(H13:H212),LEFT(CELL("format",H13:H212),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="H14:H213">
+      <formula1>AND(ISNUMBER(H14:H213),LEFT(CELL("format",H14:H213),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>